<commit_message>
goliatt sex 14 fev 2025 16:14:16 -03
</commit_message>
<xml_diff>
--- a/propp-pro-equipamentos-filtrado.xlsx
+++ b/propp-pro-equipamentos-filtrado.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
   <si>
     <t>PPG</t>
   </si>
@@ -132,6 +132,9 @@
     <t>Fotocolorímetro multiprocessado</t>
   </si>
   <si>
+    <t>Sonda multiparâmetros de qualidade de água</t>
+  </si>
+  <si>
     <t>Monitor Dell de 55” 4K para Salas de Conferência – P5525QC</t>
   </si>
   <si>
@@ -209,6 +212,14 @@
   </si>
   <si>
     <t xml:space="preserve">O equipamento permitirá a realização de projetos que assumam a água como fator ambiental central de análise, em diálogo com condições pristinas e alterações ambientais em hidrossistemas; projetos que tenham na água o elemento-chave de compreensão da dinâmica das paisagens; projetos relacionados à poluição hídrica e saúde humana.
+Professores
+Miguel Felippe - TERRA/PPGEO
+Cézar Rocha - NAGEA/PPGEO/PROAC
+Camila Neves - GEOPED/PPGEO
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O equipamento apoiará a realização de projetos que assumam a água como fator ambiental central de análise, em diálogo com condições pristinas e alterações ambientais em hidrossistemas; projetos que tenham na água o elemento-chave de compreensão da dinâmica das paisagens; projetos relacionados à poluição hídrica e saúde humana.
 Professores
 Miguel Felippe - TERRA/PPGEO
 Cézar Rocha - NAGEA/PPGEO/PROAC
@@ -622,7 +633,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -677,13 +688,13 @@
         <v>42468</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -706,13 +717,13 @@
         <v>150000</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -735,13 +746,13 @@
         <v>50000</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -764,13 +775,13 @@
         <v>38000</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -793,13 +804,13 @@
         <v>74000</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -822,10 +833,10 @@
         <v>11896.95</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -848,10 +859,10 @@
         <v>95776</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -874,10 +885,10 @@
         <v>14115</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -900,10 +911,10 @@
         <v>10200</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
         <v>13</v>
@@ -929,10 +940,10 @@
         <v>21000</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
@@ -958,18 +969,18 @@
         <v>10000</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -981,19 +992,19 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>13410</v>
+        <v>8000</v>
       </c>
       <c r="F13">
-        <v>13410</v>
+        <v>8000</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1001,7 +1012,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
@@ -1010,77 +1021,77 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>14849.1</v>
+        <v>13410</v>
       </c>
       <c r="F14">
-        <v>14849.1</v>
+        <v>13410</v>
       </c>
       <c r="G14" t="s">
         <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>21000</v>
+        <v>14849.1</v>
       </c>
       <c r="F15">
-        <v>42000</v>
+        <v>14849.1</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>13000</v>
+        <v>21000</v>
       </c>
       <c r="F16">
-        <v>65000</v>
+        <v>42000</v>
       </c>
       <c r="G16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1088,36 +1099,36 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>15000</v>
+        <v>13000</v>
       </c>
       <c r="F17">
-        <v>15000</v>
+        <v>65000</v>
       </c>
       <c r="G17" t="s">
         <v>38</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
@@ -1126,24 +1137,27 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <v>29174.9</v>
+        <v>15000</v>
       </c>
       <c r="F18">
-        <v>29174.9</v>
+        <v>15000</v>
       </c>
       <c r="G18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="I18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
         <v>36</v>
@@ -1152,19 +1166,45 @@
         <v>1</v>
       </c>
       <c r="E19">
+        <v>29174.9</v>
+      </c>
+      <c r="F19">
+        <v>29174.9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
         <v>122678.94</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>122678.94</v>
       </c>
-      <c r="G19" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" t="s">
-        <v>67</v>
+      <c r="G20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>